<commit_message>
Error a explode (JODER!!!!!)
</commit_message>
<xml_diff>
--- a/prova.xlsx
+++ b/prova.xlsx
@@ -473,7 +473,7 @@
       <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
-          <t>['A veure què tal']</t>
+          <t>['gfdhgfdhgf']</t>
         </is>
       </c>
       <c r="E2" t="inlineStr"/>
@@ -485,8 +485,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>['Té molta tonteria' 'asdfsadf' 'gdfgdfs' 'ge'
- 'klfhldskhflsdhflkdshflsdhflkdslksada,sdmsa,dms,dmsa' 'xxcvcxv']</t>
+          <t>['shhfgdhgf']</t>
         </is>
       </c>
       <c r="C3" t="inlineStr"/>

</xml_diff>